<commit_message>
touch up + clean up
</commit_message>
<xml_diff>
--- a/Tender/EmailTemplate.xlsx
+++ b/Tender/EmailTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Documents\UiPath\Tender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Desktop\RPA Project\UiPathPractice\Tender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868B1A7C-7D6E-4A19-9969-47BF1B8A8424}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4565C152-2019-46EC-8F39-9712FDA2CF79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -72,7 +72,14 @@
     <t>xiaodiz572@hotmail.com</t>
   </si>
   <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>zephytk@gmail.com</t>
+  </si>
+  <si>
     <t>This is the start of email body message
+Workflow Version 5
 Team Charlie Rocks
 This is  a bot generated message.
 regards</t>
@@ -441,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E9B932-F46E-4292-B019-FC95463D2DDD}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -452,11 +459,11 @@
     <col min="1" max="1" width="6.08203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="61.08203125" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="61.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,10 +477,13 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -486,103 +496,107 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E24" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:E24"/>
+    <mergeCell ref="F2:F24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FBB74F0F-5572-4568-B26E-53B5E8BC5E74}"/>
     <hyperlink ref="B3:B5" r:id="rId2" display="xiaodiz572@hotmail.com" xr:uid="{C3D65DF4-7D84-431C-BB60-949EA85A5947}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{F1C875B4-CDC9-493B-815A-088A7212AAB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added close application window at end of workflow
</commit_message>
<xml_diff>
--- a/Tender/EmailTemplate.xlsx
+++ b/Tender/EmailTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Desktop\RPA Project\UiPathPractice\Tender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4565C152-2019-46EC-8F39-9712FDA2CF79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BFAEA6-8722-407F-B127-4D4ABA5122AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
   </bookViews>
@@ -78,10 +78,7 @@
     <t>zephytk@gmail.com</t>
   </si>
   <si>
-    <t>This is the start of email body message
-Workflow Version 5
-Team Charlie Rocks
-This is  a bot generated message.
+    <t>This email is sent by an UiPath Orchestrator Unattended bot.
 regards</t>
   </si>
 </sst>
@@ -131,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -451,7 +448,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -483,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -588,9 +585,6 @@
       <c r="F24" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F2:F24"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FBB74F0F-5572-4568-B26E-53B5E8BC5E74}"/>
     <hyperlink ref="B3:B5" r:id="rId2" display="xiaodiz572@hotmail.com" xr:uid="{C3D65DF4-7D84-431C-BB60-949EA85A5947}"/>

</xml_diff>